<commit_message>
Update sample final tests
</commit_message>
<xml_diff>
--- a/IT002-OOP/it002m21mmcl/it002m21mmcl2.xlsx
+++ b/IT002-OOP/it002m21mmcl/it002m21mmcl2.xlsx
@@ -475,7 +475,9 @@
       <c r="D2" t="n">
         <v>275</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>800</v>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
     </row>
@@ -524,7 +526,9 @@
       <c r="D5" t="n">
         <v>300</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>600</v>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
     </row>
@@ -543,7 +547,9 @@
       <c r="D6" t="n">
         <v>800</v>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>650</v>
+      </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
     </row>
@@ -575,7 +581,9 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>400</v>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
     </row>
@@ -594,7 +602,9 @@
       <c r="D9" t="n">
         <v>800</v>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>700</v>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
     </row>
@@ -613,7 +623,9 @@
       <c r="D10" t="n">
         <v>600</v>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>400</v>
+      </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
     </row>
@@ -651,7 +663,9 @@
       <c r="D12" t="n">
         <v>600</v>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>600</v>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
     </row>
@@ -670,7 +684,9 @@
       <c r="D13" t="n">
         <v>800</v>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>600</v>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
     </row>
@@ -689,7 +705,9 @@
       <c r="D14" t="n">
         <v>800</v>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>800</v>
+      </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
     </row>
@@ -708,7 +726,9 @@
       <c r="D15" t="n">
         <v>642.86</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>650</v>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
     </row>
@@ -757,7 +777,9 @@
       <c r="D18" t="n">
         <v>500</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>700</v>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
     </row>
@@ -774,7 +796,9 @@
       <c r="D19" t="n">
         <v>100</v>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>400</v>
+      </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
     </row>
@@ -793,7 +817,9 @@
       <c r="D20" t="n">
         <v>800</v>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>500</v>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
     </row>
@@ -812,7 +838,9 @@
       <c r="D21" t="n">
         <v>800</v>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>700</v>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
     </row>
@@ -831,7 +859,9 @@
       <c r="D22" t="n">
         <v>800</v>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>800</v>
+      </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
     </row>
@@ -850,7 +880,9 @@
       <c r="D23" t="n">
         <v>500</v>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>800</v>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
     </row>

</xml_diff>